<commit_message>
changes during the meeting
</commit_message>
<xml_diff>
--- a/code/pdf/data_cult_empl_fig.xlsx
+++ b/code/pdf/data_cult_empl_fig.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F106"/>
+  <dimension ref="A1:F109"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -3293,6 +3293,72 @@
         <v>-3.557548579970097</v>
       </c>
     </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>THS_PERS</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t xml:space="preserve">  </t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>THS_PERS</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   </t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>THS_PERS</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>2022</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>